<commit_message>
fixed weird bug in Cavg1 calculation - ensure tau is not in model file; now model matches theory better; for Ateoz, set keS1 and keS3 to 1 instead of 0
</commit_message>
<xml_diff>
--- a/data/ModelF_Atezolizumab_Params.xlsx
+++ b/data/ModelF_Atezolizumab_Params.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28702"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="200" yWindow="1240" windowWidth="26960" windowHeight="16280" tabRatio="500"/>
+    <workbookView xWindow="1240" yWindow="2620" windowWidth="15200" windowHeight="16280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -887,207 +887,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="32">
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF800000"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1348,6 +1147,207 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF800000"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
@@ -1368,21 +1368,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J79" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J79" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:J79"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="Order" dataDxfId="29"/>
-    <tableColumn id="2" name="ParamType" dataDxfId="28"/>
-    <tableColumn id="3" name="Molecule" dataDxfId="27"/>
-    <tableColumn id="4" name="Description" dataDxfId="26"/>
-    <tableColumn id="5" name="Parameter" dataDxfId="25"/>
-    <tableColumn id="6" name="Value" dataDxfId="24"/>
-    <tableColumn id="7" name="Units" dataDxfId="23"/>
-    <tableColumn id="8" name="Source" dataDxfId="22"/>
-    <tableColumn id="10" name="Formula" dataDxfId="21">
+    <tableColumn id="1" name="Order" dataDxfId="9"/>
+    <tableColumn id="2" name="ParamType" dataDxfId="8"/>
+    <tableColumn id="3" name="Molecule" dataDxfId="7"/>
+    <tableColumn id="4" name="Description" dataDxfId="6"/>
+    <tableColumn id="5" name="Parameter" dataDxfId="5"/>
+    <tableColumn id="6" name="Value" dataDxfId="4"/>
+    <tableColumn id="7" name="Units" dataDxfId="3"/>
+    <tableColumn id="8" name="Source" dataDxfId="2"/>
+    <tableColumn id="10" name="Formula" dataDxfId="1">
       <calculatedColumnFormula>_xlfn.IFNA(_xlfn.FORMULATEXT(F2),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Comment or Reference" dataDxfId="20"/>
+    <tableColumn id="9" name="Comment or Reference" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1712,8 +1712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="99" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2654,13 +2654,13 @@
         <v>33</v>
       </c>
       <c r="F29" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I29" s="14" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -2687,13 +2687,13 @@
         <v>35</v>
       </c>
       <c r="F30" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I30" s="14" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -4274,82 +4274,82 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F293">
-    <cfRule type="containsText" dxfId="19" priority="30" operator="containsText" text="derived">
+    <cfRule type="containsText" dxfId="31" priority="30" operator="containsText" text="derived">
       <formula>NOT(ISERROR(SEARCH("derived",F293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="expression" dxfId="18" priority="28">
+    <cfRule type="expression" dxfId="30" priority="28">
       <formula>$H2="fit"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55:I58 K55:K58 D58 C55:C58 J25:J28 K24:K28 K31:K34 I24:J24 G35:G36 H24:I38 B53:K53 B47:H52 I37:I66 A1:K3 C37:G38 C24:G30 B24:B46 C59:K66 C54:K54 A80:K1048576 B69:H72 B54:B68 B4:K23 A79:H79 C67:H68 J29:K30 C39:H46 J35:K52 C35:E36 I67:K79 A4:A77">
-    <cfRule type="containsText" dxfId="17" priority="27" operator="containsText" text="calc">
+    <cfRule type="containsText" dxfId="29" priority="27" operator="containsText" text="calc">
       <formula>NOT(ISERROR(SEARCH("calc",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H80:I1048576 H79 H67:H72 H1:I66 I67:I79">
-    <cfRule type="containsText" dxfId="16" priority="25" operator="containsText" text="literature">
+    <cfRule type="containsText" dxfId="28" priority="25" operator="containsText" text="literature">
       <formula>NOT(ISERROR(SEARCH("literature",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="26" operator="containsText" text="guess">
+    <cfRule type="containsText" dxfId="27" priority="26" operator="containsText" text="guess">
       <formula>NOT(ISERROR(SEARCH("guess",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53:I66 H1:I38 I37:I52 H80:I1048576 H79 H67:H72 H39:H52 I67:I79">
-    <cfRule type="containsText" dxfId="14" priority="20" operator="containsText" text="not used">
+    <cfRule type="containsText" dxfId="26" priority="20" operator="containsText" text="not used">
       <formula>NOT(ISERROR(SEARCH("not used",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="21" operator="containsText" text="literature">
+    <cfRule type="containsText" dxfId="25" priority="21" operator="containsText" text="literature">
       <formula>NOT(ISERROR(SEARCH("literature",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="22" operator="containsText" text="guess">
+    <cfRule type="containsText" dxfId="24" priority="22" operator="containsText" text="guess">
       <formula>NOT(ISERROR(SEARCH("guess",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="23" operator="containsText" text="calc">
+    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="calc">
       <formula>NOT(ISERROR(SEARCH("calc",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="24" operator="containsText" text="check">
+    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="check">
       <formula>NOT(ISERROR(SEARCH("check",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H79:H1048576 H1:H72">
-    <cfRule type="containsText" dxfId="9" priority="19" operator="containsText" text="internal data">
+    <cfRule type="containsText" dxfId="21" priority="19" operator="containsText" text="internal data">
       <formula>NOT(ISERROR(SEARCH("internal data",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73:H77">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="calc">
+    <cfRule type="containsText" dxfId="20" priority="9" operator="containsText" text="calc">
       <formula>NOT(ISERROR(SEARCH("calc",H73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73:H77">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="literature">
+    <cfRule type="containsText" dxfId="19" priority="7" operator="containsText" text="literature">
       <formula>NOT(ISERROR(SEARCH("literature",H73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="guess">
+    <cfRule type="containsText" dxfId="18" priority="8" operator="containsText" text="guess">
       <formula>NOT(ISERROR(SEARCH("guess",H73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73:H77">
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="not used">
+    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="not used">
       <formula>NOT(ISERROR(SEARCH("not used",H73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="literature">
+    <cfRule type="containsText" dxfId="16" priority="3" operator="containsText" text="literature">
       <formula>NOT(ISERROR(SEARCH("literature",H73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="guess">
+    <cfRule type="containsText" dxfId="15" priority="4" operator="containsText" text="guess">
       <formula>NOT(ISERROR(SEARCH("guess",H73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="calc">
+    <cfRule type="containsText" dxfId="14" priority="5" operator="containsText" text="calc">
       <formula>NOT(ISERROR(SEARCH("calc",H73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="check">
+    <cfRule type="containsText" dxfId="13" priority="6" operator="containsText" text="check">
       <formula>NOT(ISERROR(SEARCH("check",H73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73:H77">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="internal data">
+    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="internal data">
       <formula>NOT(ISERROR(SEARCH("internal data",H73)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
setting keS3 and keDS3 = 0 instead of 1
</commit_message>
<xml_diff>
--- a/data/ModelF_Atezolizumab_Params.xlsx
+++ b/data/ModelF_Atezolizumab_Params.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steinanf/GitHub/IMA_TumorModeling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/astein/Github/TumorModelingCode/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1240" yWindow="2620" windowWidth="15200" windowHeight="16280" tabRatio="500"/>
+    <workbookView xWindow="1240" yWindow="460" windowWidth="15200" windowHeight="14960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1712,8 +1712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="99" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="99" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2654,13 +2654,13 @@
         <v>33</v>
       </c>
       <c r="F29" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I29" s="14" t="str">
         <f t="shared" ca="1" si="1"/>
@@ -2687,13 +2687,13 @@
         <v>35</v>
       </c>
       <c r="F30" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I30" s="14" t="str">
         <f t="shared" ca="1" si="1"/>

</xml_diff>

<commit_message>
adding in Thiele modulus calculation for Herceptin and tweaking it for Pembro and Atezo
</commit_message>
<xml_diff>
--- a/data/ModelF_Atezolizumab_Params.xlsx
+++ b/data/ModelF_Atezolizumab_Params.xlsx
@@ -37,6 +37,7 @@
     <definedName name="Kd">Sheet1!$F$18</definedName>
     <definedName name="keD">Sheet1!$F$5</definedName>
     <definedName name="keD3_">Sheet1!$F$52</definedName>
+    <definedName name="keDM3">Sheet1!$F$42</definedName>
     <definedName name="keDMtot">Sheet1!$F$76</definedName>
     <definedName name="keDS1">Sheet1!$F$26</definedName>
     <definedName name="keM">Sheet1!$F$76</definedName>
@@ -45,6 +46,7 @@
     <definedName name="kon">Sheet1!$F$21</definedName>
     <definedName name="kshed">Sheet1!$F$45</definedName>
     <definedName name="kshedDM1">Sheet1!$F$44</definedName>
+    <definedName name="kshedDM3">Sheet1!$F$46</definedName>
     <definedName name="kshedM1">Sheet1!$F$43</definedName>
     <definedName name="kshedM3">Sheet1!$F$45</definedName>
     <definedName name="M10_">Sheet1!$F$35</definedName>
@@ -1713,8 +1715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="99" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="99" workbookViewId="0">
+      <selection activeCell="F77" sqref="F77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4195,7 +4197,7 @@
         <v>195</v>
       </c>
       <c r="F76" s="3">
-        <f>F46+F42</f>
+        <f>kshedDM3+keDM3</f>
         <v>3</v>
       </c>
       <c r="G76" s="2" t="s">
@@ -4206,7 +4208,7 @@
       </c>
       <c r="I76" s="12" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>=F46+F42</v>
+        <v>=kshedDM3+keDM3</v>
       </c>
       <c r="J76" s="10"/>
     </row>

</xml_diff>

<commit_message>
fixing params (Pembro was 60 keDM3 instead of 6)
</commit_message>
<xml_diff>
--- a/data/ModelF_Atezolizumab_Params.xlsx
+++ b/data/ModelF_Atezolizumab_Params.xlsx
@@ -1715,8 +1715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="99" workbookViewId="0">
-      <selection activeCell="F77" sqref="F77"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="99" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3142,7 +3142,7 @@
         <v>97</v>
       </c>
       <c r="F44" s="13">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G44" s="18" t="s">
         <v>4</v>
@@ -3206,7 +3206,7 @@
       </c>
       <c r="F46" s="3">
         <f>kshedDM1</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>4</v>
@@ -4198,7 +4198,7 @@
       </c>
       <c r="F76" s="3">
         <f>kshedDM3+keDM3</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>4</v>
@@ -4230,7 +4230,7 @@
       </c>
       <c r="F77" s="16">
         <f>keDMtot*M30_/(k31D_thurber*Cavg)</f>
-        <v>1.5960519921725189E-2</v>
+        <v>3.1921039843450377E-2</v>
       </c>
       <c r="G77" s="17" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
tweaked data to highlight where guess was for B
</commit_message>
<xml_diff>
--- a/data/ModelF_Atezolizumab_Params.xlsx
+++ b/data/ModelF_Atezolizumab_Params.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steinanf/GitHub/TumorModeling_IMA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3051FD91-6DA8-EB41-B43D-AFEA0AE729E9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8460" yWindow="460" windowWidth="24100" windowHeight="18080" tabRatio="500"/>
+    <workbookView xWindow="4700" yWindow="460" windowWidth="24100" windowHeight="16900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -77,7 +78,7 @@
     <definedName name="VtumDS">Sheet1!$F$49</definedName>
     <definedName name="VtumS">Sheet1!$F$48</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -90,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="200">
   <si>
     <t>Parameter</t>
   </si>
@@ -687,12 +688,15 @@
   </si>
   <si>
     <t>From Thurber08 - 10.1016/j.addr.2008.04.012</t>
+  </si>
+  <si>
+    <t>calc/guess</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1371,21 +1375,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:J79" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J79"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J79" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J79" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" name="Order" dataDxfId="9"/>
-    <tableColumn id="2" name="ParamType" dataDxfId="8"/>
-    <tableColumn id="3" name="Molecule" dataDxfId="7"/>
-    <tableColumn id="4" name="Description" dataDxfId="6"/>
-    <tableColumn id="5" name="Parameter" dataDxfId="5"/>
-    <tableColumn id="6" name="Value" dataDxfId="4"/>
-    <tableColumn id="7" name="Units" dataDxfId="3"/>
-    <tableColumn id="8" name="Source" dataDxfId="2"/>
-    <tableColumn id="10" name="Formula" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Order" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ParamType" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Molecule" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Parameter" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Value" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Units" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Source" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Formula" dataDxfId="1">
       <calculatedColumnFormula>_xlfn.IFNA(_xlfn.FORMULATEXT(F2),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Comment or Reference" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Comment or Reference" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1712,11 +1716,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" zoomScale="99" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3830,21 +3834,21 @@
       <c r="E65" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F65" s="3">
+      <c r="F65" s="13">
         <f>VD1_/VD3_*k13d_prop*3</f>
         <v>0.45123966942148763</v>
       </c>
-      <c r="G65" s="2" t="s">
+      <c r="G65" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="H65" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I65" s="14" t="str">
+      <c r="H65" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="I65" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
         <v>=VD1_/VD3_*k13d_prop*3</v>
       </c>
-      <c r="J65" s="9" t="s">
+      <c r="J65" s="19" t="s">
         <v>148</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Use Ayyar18 for lymphocyte trafficking
</commit_message>
<xml_diff>
--- a/data/ModelF_Atezolizumab_Params.xlsx
+++ b/data/ModelF_Atezolizumab_Params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steinanf/GitHub/TumorModeling_IMA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3051FD91-6DA8-EB41-B43D-AFEA0AE729E9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E230CC-4662-C54A-8F0D-2BFDC454D006}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4700" yWindow="460" windowWidth="24100" windowHeight="16900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -639,12 +639,6 @@
     <t>scale by volume</t>
   </si>
   <si>
-    <t>Could be much faster, or could not occur at all depending on tissue</t>
-  </si>
-  <si>
-    <t>scale by volume such that at equilibrium, the amount flowing back and forth are equal</t>
-  </si>
-  <si>
     <t>Dose</t>
   </si>
   <si>
@@ -691,6 +685,12 @@
   </si>
   <si>
     <t>calc/guess</t>
+  </si>
+  <si>
+    <t>Ayyar18, Table 4 kin https://doi.org/10.1007/s10928-018-9585-x(012 345678,9-().volV)(0123456789().,-volV)</t>
+  </si>
+  <si>
+    <t>Ayyar18, Table 4 kout https://doi.org/10.1007/s10928-018-9585-x(012 345678,9-().volV)(0123456789().,-volV)</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -864,9 +864,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -893,7 +890,97 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="41">
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1375,21 +1462,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J79" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J79" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="A1:J79" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Order" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ParamType" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Molecule" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Parameter" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Value" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Units" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Source" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Formula" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Order" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ParamType" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Molecule" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Parameter" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Value" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Units" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Source" dataDxfId="11"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Formula" dataDxfId="10">
       <calculatedColumnFormula>_xlfn.IFNA(_xlfn.FORMULATEXT(F2),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Comment or Reference" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Comment or Reference" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1720,7 +1807,7 @@
   <dimension ref="A1:J79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" zoomScale="99" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3815,7 +3902,7 @@
         <v>=2*P*Rcap/Rkrogh^2</v>
       </c>
       <c r="J64" s="15" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="65" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -3842,7 +3929,7 @@
         <v>4</v>
       </c>
       <c r="H65" s="18" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I65" s="22" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -3970,21 +4057,22 @@
       <c r="E69" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F69" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="G69" s="18" t="s">
+      <c r="F69" s="3">
+        <f>0.002*24</f>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="G69" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H69" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="I69" s="19" t="str">
+      <c r="H69" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I69" s="12" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="J69" s="25" t="s">
-        <v>182</v>
+        <v>=0.002*24</v>
+      </c>
+      <c r="J69" s="15" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="70" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.2">
@@ -4004,21 +4092,21 @@
         <v>101</v>
       </c>
       <c r="F70" s="3">
-        <f>k13M*VD1_/VD3_</f>
-        <v>6.56</v>
+        <f>0.23*24</f>
+        <v>5.5200000000000005</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>4</v>
       </c>
       <c r="H70" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I70" s="12" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v>=k13M*VD1_/VD3_</v>
+        <v>=0.23*24</v>
       </c>
       <c r="J70" s="12" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
     </row>
     <row r="71" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -4039,7 +4127,7 @@
       </c>
       <c r="F71" s="3">
         <f>k13M</f>
-        <v>0.2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>4</v>
@@ -4071,7 +4159,7 @@
       </c>
       <c r="F72" s="3">
         <f>k31M</f>
-        <v>6.56</v>
+        <v>5.5200000000000005</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>4</v>
@@ -4092,23 +4180,23 @@
         <v>72</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C73" s="8" t="s">
         <v>68</v>
       </c>
       <c r="D73" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F73" s="3">
         <f>1200*6.67</f>
         <v>8004</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H73" s="2" t="s">
         <v>53</v>
@@ -4118,7 +4206,7 @@
         <v>=1200*6.67</v>
       </c>
       <c r="J73" s="9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="74" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -4126,22 +4214,22 @@
         <v>73</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C74" s="8" t="s">
         <v>68</v>
       </c>
       <c r="D74" s="8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="F74" s="3">
         <v>21</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H74" s="2" t="s">
         <v>53</v>
@@ -4163,10 +4251,10 @@
         <v>68</v>
       </c>
       <c r="D75" s="8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F75" s="3">
         <f>Dose/(CL*Tau)</f>
@@ -4195,10 +4283,10 @@
         <v>81</v>
       </c>
       <c r="D76" s="8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F76" s="3">
         <f>kshedDM3+keDM3</f>
@@ -4227,10 +4315,10 @@
         <v>81</v>
       </c>
       <c r="D77" s="8" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F77" s="16">
         <f>keDMtot*M30_/(k31D_thurber*Cavg)</f>
@@ -4240,14 +4328,14 @@
         <v>3</v>
       </c>
       <c r="H77" s="17" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="I77" s="21" t="str">
         <f t="shared" ca="1" si="2"/>
         <v>=keDMtot*M30_/(k31D_thurber*Cavg)</v>
       </c>
       <c r="J77" s="9" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="78" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
@@ -4280,83 +4368,118 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F293">
-    <cfRule type="containsText" dxfId="31" priority="30" operator="containsText" text="derived">
+    <cfRule type="containsText" dxfId="40" priority="39" operator="containsText" text="derived">
       <formula>NOT(ISERROR(SEARCH("derived",F293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="expression" dxfId="30" priority="28">
+    <cfRule type="expression" dxfId="39" priority="37">
       <formula>$H2="fit"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H55:I58 K55:K58 D58 C55:C58 J25:J28 K24:K28 K31:K34 I24:J24 G35:G36 H24:I38 B53:K53 B47:H52 I37:I66 A1:K3 C37:G38 C24:G30 B24:B46 C59:K66 C54:K54 A80:K1048576 B69:H72 B54:B68 B4:K23 A79:H79 C67:H68 J29:K30 C39:H46 J35:K52 C35:E36 I67:K79 A4:A77">
-    <cfRule type="containsText" dxfId="29" priority="27" operator="containsText" text="calc">
+  <conditionalFormatting sqref="H55:I58 K55:K58 D58 C55:C58 J25:J28 K24:K28 K31:K34 I24:J24 G35:G36 H24:I38 B53:K53 B47:H52 I37:I66 A1:K3 C37:G38 C24:G30 B24:B46 C54:K54 A80:K1048576 B71:H72 B54:B68 B4:K23 A79:H79 J29:K30 C39:H46 J35:K52 C35:E36 C59:K68 A4:A77 I71:K79 K69:K70 B69:C70">
+    <cfRule type="containsText" dxfId="38" priority="36" operator="containsText" text="calc">
       <formula>NOT(ISERROR(SEARCH("calc",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H80:I1048576 H79 H67:H72 H1:I66 I67:I79">
-    <cfRule type="containsText" dxfId="28" priority="25" operator="containsText" text="literature">
+  <conditionalFormatting sqref="H80:I1048576 H79 H1:I68 I71:I79 H71:H72">
+    <cfRule type="containsText" dxfId="37" priority="34" operator="containsText" text="literature">
       <formula>NOT(ISERROR(SEARCH("literature",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="26" operator="containsText" text="guess">
+    <cfRule type="containsText" dxfId="36" priority="35" operator="containsText" text="guess">
       <formula>NOT(ISERROR(SEARCH("guess",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H53:I66 H1:I38 I37:I52 H80:I1048576 H79 H67:H72 H39:H52 I67:I79">
-    <cfRule type="containsText" dxfId="26" priority="20" operator="containsText" text="not used">
+  <conditionalFormatting sqref="H1:I38 I37:I52 H80:I1048576 H79 H39:H52 H53:I68 I71:I79 H71:H72">
+    <cfRule type="containsText" dxfId="35" priority="29" operator="containsText" text="not used">
       <formula>NOT(ISERROR(SEARCH("not used",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="21" operator="containsText" text="literature">
+    <cfRule type="containsText" dxfId="34" priority="30" operator="containsText" text="literature">
       <formula>NOT(ISERROR(SEARCH("literature",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="22" operator="containsText" text="guess">
+    <cfRule type="containsText" dxfId="33" priority="31" operator="containsText" text="guess">
       <formula>NOT(ISERROR(SEARCH("guess",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="calc">
+    <cfRule type="containsText" dxfId="32" priority="32" operator="containsText" text="calc">
       <formula>NOT(ISERROR(SEARCH("calc",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="check">
+    <cfRule type="containsText" dxfId="31" priority="33" operator="containsText" text="check">
       <formula>NOT(ISERROR(SEARCH("check",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H79:H1048576 H1:H72">
-    <cfRule type="containsText" dxfId="21" priority="19" operator="containsText" text="internal data">
+  <conditionalFormatting sqref="H79:H1048576 H1:H68 H71:H72">
+    <cfRule type="containsText" dxfId="30" priority="28" operator="containsText" text="internal data">
       <formula>NOT(ISERROR(SEARCH("internal data",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73:H77">
-    <cfRule type="containsText" dxfId="20" priority="9" operator="containsText" text="calc">
+    <cfRule type="containsText" dxfId="29" priority="18" operator="containsText" text="calc">
       <formula>NOT(ISERROR(SEARCH("calc",H73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73:H77">
-    <cfRule type="containsText" dxfId="19" priority="7" operator="containsText" text="literature">
+    <cfRule type="containsText" dxfId="28" priority="16" operator="containsText" text="literature">
       <formula>NOT(ISERROR(SEARCH("literature",H73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="8" operator="containsText" text="guess">
+    <cfRule type="containsText" dxfId="27" priority="17" operator="containsText" text="guess">
       <formula>NOT(ISERROR(SEARCH("guess",H73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73:H77">
-    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="not used">
+    <cfRule type="containsText" dxfId="26" priority="11" operator="containsText" text="not used">
       <formula>NOT(ISERROR(SEARCH("not used",H73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="3" operator="containsText" text="literature">
+    <cfRule type="containsText" dxfId="25" priority="12" operator="containsText" text="literature">
       <formula>NOT(ISERROR(SEARCH("literature",H73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="4" operator="containsText" text="guess">
+    <cfRule type="containsText" dxfId="24" priority="13" operator="containsText" text="guess">
       <formula>NOT(ISERROR(SEARCH("guess",H73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="5" operator="containsText" text="calc">
+    <cfRule type="containsText" dxfId="23" priority="14" operator="containsText" text="calc">
       <formula>NOT(ISERROR(SEARCH("calc",H73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="6" operator="containsText" text="check">
+    <cfRule type="containsText" dxfId="22" priority="15" operator="containsText" text="check">
       <formula>NOT(ISERROR(SEARCH("check",H73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73:H77">
-    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="internal data">
+    <cfRule type="containsText" dxfId="21" priority="10" operator="containsText" text="internal data">
       <formula>NOT(ISERROR(SEARCH("internal data",H73)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D69:J70">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="calc">
+      <formula>NOT(ISERROR(SEARCH("calc",D69)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H69:I70">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="literature">
+      <formula>NOT(ISERROR(SEARCH("literature",H69)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="guess">
+      <formula>NOT(ISERROR(SEARCH("guess",H69)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H69:I70">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="not used">
+      <formula>NOT(ISERROR(SEARCH("not used",H69)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="literature">
+      <formula>NOT(ISERROR(SEARCH("literature",H69)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="guess">
+      <formula>NOT(ISERROR(SEARCH("guess",H69)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="calc">
+      <formula>NOT(ISERROR(SEARCH("calc",H69)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="check">
+      <formula>NOT(ISERROR(SEARCH("check",H69)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H69:H70">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="internal data">
+      <formula>NOT(ISERROR(SEARCH("internal data",H69)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
implementing code for changing V all at once
</commit_message>
<xml_diff>
--- a/data/ModelF_Atezolizumab_Params.xlsx
+++ b/data/ModelF_Atezolizumab_Params.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11015"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steinanf/GitHub/TumorModeling_IMA/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E230CC-4662-C54A-8F0D-2BFDC454D006}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33946ADF-79D2-7540-99FD-119DC8CABCE5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4700" yWindow="460" windowWidth="24100" windowHeight="16900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
     <definedName name="VtumDS">Sheet1!$F$49</definedName>
     <definedName name="VtumS">Sheet1!$F$48</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -91,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="206">
   <si>
     <t>Parameter</t>
   </si>
@@ -691,13 +691,31 @@
   </si>
   <si>
     <t>Ayyar18, Table 4 kout https://doi.org/10.1007/s10928-018-9585-x(012 345678,9-().volV)(0123456789().,-volV)</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Tissue Volume</t>
+  </si>
+  <si>
+    <t>used for Vlink model</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -733,6 +751,12 @@
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -790,7 +814,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -864,6 +888,18 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -890,7 +926,187 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="68">
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="4" tint="-0.499984740745262"/>
@@ -1240,6 +1456,96 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1462,21 +1768,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J79" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A1:J79" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:J80" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+  <autoFilter ref="A1:J80" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Order" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ParamType" dataDxfId="17"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Molecule" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Parameter" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Value" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Units" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Source" dataDxfId="11"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Formula" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Order" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="ParamType" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Molecule" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Description" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Parameter" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Value" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Units" dataDxfId="30"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Source" dataDxfId="29"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Formula" dataDxfId="28">
       <calculatedColumnFormula>_xlfn.IFNA(_xlfn.FORMULATEXT(F2),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Comment or Reference" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Comment or Reference" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1804,10 +2110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J79"/>
+  <dimension ref="A1:J80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="99" workbookViewId="0">
-      <selection activeCell="D64" sqref="D64"/>
+    <sheetView tabSelected="1" topLeftCell="A60" zoomScale="99" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78:XFD80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4339,147 +4645,326 @@
       </c>
     </row>
     <row r="78" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="8"/>
-      <c r="B78" s="8"/>
-      <c r="C78" s="8"/>
-      <c r="D78" s="8"/>
-      <c r="E78" s="2"/>
-      <c r="F78" s="3"/>
-      <c r="G78" s="2"/>
-      <c r="H78" s="2"/>
+      <c r="A78" s="8">
+        <v>77</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F78" s="3">
+        <f>VD1_</f>
+        <v>3.28</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="I78" s="12" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="J78" s="9"/>
+        <v>=VD1_</v>
+      </c>
+      <c r="J78" s="9" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A79" s="8"/>
-      <c r="B79" s="8"/>
-      <c r="C79" s="8"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="2"/>
-      <c r="G79" s="2"/>
+      <c r="A79" s="8">
+        <v>78</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F79" s="3">
+        <f>VD2_</f>
+        <v>3.63</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="I79" s="12" t="str">
         <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="J79" s="9"/>
+        <v>=VD2_</v>
+      </c>
+      <c r="J79" s="9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A80" s="25">
+        <v>79</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="E80" s="26" t="s">
+        <v>202</v>
+      </c>
+      <c r="F80" s="27">
+        <f>VD3_</f>
+        <v>0.1</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I80" s="28" t="str">
+        <f ca="1">_xlfn.IFNA(_xlfn.FORMULATEXT(F80),"")</f>
+        <v>=VD3_</v>
+      </c>
+      <c r="J80" s="9" t="s">
+        <v>205</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F293">
-    <cfRule type="containsText" dxfId="40" priority="39" operator="containsText" text="derived">
+    <cfRule type="containsText" dxfId="67" priority="66" operator="containsText" text="derived">
       <formula>NOT(ISERROR(SEARCH("derived",F293)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J8">
-    <cfRule type="expression" dxfId="39" priority="37">
+    <cfRule type="expression" dxfId="66" priority="64">
       <formula>$H2="fit"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H55:I58 K55:K58 D58 C55:C58 J25:J28 K24:K28 K31:K34 I24:J24 G35:G36 H24:I38 B53:K53 B47:H52 I37:I66 A1:K3 C37:G38 C24:G30 B24:B46 C54:K54 A80:K1048576 B71:H72 B54:B68 B4:K23 A79:H79 J29:K30 C39:H46 J35:K52 C35:E36 C59:K68 A4:A77 I71:K79 K69:K70 B69:C70">
-    <cfRule type="containsText" dxfId="38" priority="36" operator="containsText" text="calc">
+  <conditionalFormatting sqref="H55:I58 K55:K58 D58 C55:C58 J25:J28 K24:K28 K31:K34 I24:J24 G35:G36 H24:I38 B53:K53 B47:H52 I37:I66 A1:K3 C37:G38 C24:G30 B24:B46 C54:K54 A81:K1048576 B71:H72 B54:B68 B4:K23 J29:K30 C39:H46 J35:K52 C35:E36 C59:K68 A4:A77 K69:K70 B69:C70 A79:G80 I71:K80">
+    <cfRule type="containsText" dxfId="65" priority="63" operator="containsText" text="calc">
       <formula>NOT(ISERROR(SEARCH("calc",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H80:I1048576 H79 H1:I68 I71:I79 H71:H72">
-    <cfRule type="containsText" dxfId="37" priority="34" operator="containsText" text="literature">
+  <conditionalFormatting sqref="H81:I1048576 H1:I68 H71:H72 I71:I80">
+    <cfRule type="containsText" dxfId="64" priority="61" operator="containsText" text="literature">
       <formula>NOT(ISERROR(SEARCH("literature",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="35" operator="containsText" text="guess">
+    <cfRule type="containsText" dxfId="63" priority="62" operator="containsText" text="guess">
       <formula>NOT(ISERROR(SEARCH("guess",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:I38 I37:I52 H80:I1048576 H79 H39:H52 H53:I68 I71:I79 H71:H72">
-    <cfRule type="containsText" dxfId="35" priority="29" operator="containsText" text="not used">
+  <conditionalFormatting sqref="H1:I38 I37:I52 H81:I1048576 H39:H52 H53:I68 H71:H72 I71:I80">
+    <cfRule type="containsText" dxfId="62" priority="56" operator="containsText" text="not used">
       <formula>NOT(ISERROR(SEARCH("not used",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="30" operator="containsText" text="literature">
+    <cfRule type="containsText" dxfId="61" priority="57" operator="containsText" text="literature">
       <formula>NOT(ISERROR(SEARCH("literature",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="31" operator="containsText" text="guess">
+    <cfRule type="containsText" dxfId="60" priority="58" operator="containsText" text="guess">
       <formula>NOT(ISERROR(SEARCH("guess",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="32" operator="containsText" text="calc">
+    <cfRule type="containsText" dxfId="59" priority="59" operator="containsText" text="calc">
       <formula>NOT(ISERROR(SEARCH("calc",H1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="33" operator="containsText" text="check">
+    <cfRule type="containsText" dxfId="58" priority="60" operator="containsText" text="check">
       <formula>NOT(ISERROR(SEARCH("check",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H79:H1048576 H1:H68 H71:H72">
-    <cfRule type="containsText" dxfId="30" priority="28" operator="containsText" text="internal data">
+  <conditionalFormatting sqref="H81:H1048576 H1:H68 H71:H72">
+    <cfRule type="containsText" dxfId="57" priority="55" operator="containsText" text="internal data">
       <formula>NOT(ISERROR(SEARCH("internal data",H1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73:H77">
-    <cfRule type="containsText" dxfId="29" priority="18" operator="containsText" text="calc">
+    <cfRule type="containsText" dxfId="56" priority="45" operator="containsText" text="calc">
       <formula>NOT(ISERROR(SEARCH("calc",H73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73:H77">
-    <cfRule type="containsText" dxfId="28" priority="16" operator="containsText" text="literature">
+    <cfRule type="containsText" dxfId="55" priority="43" operator="containsText" text="literature">
       <formula>NOT(ISERROR(SEARCH("literature",H73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="17" operator="containsText" text="guess">
+    <cfRule type="containsText" dxfId="54" priority="44" operator="containsText" text="guess">
       <formula>NOT(ISERROR(SEARCH("guess",H73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73:H77">
-    <cfRule type="containsText" dxfId="26" priority="11" operator="containsText" text="not used">
+    <cfRule type="containsText" dxfId="53" priority="38" operator="containsText" text="not used">
       <formula>NOT(ISERROR(SEARCH("not used",H73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="12" operator="containsText" text="literature">
+    <cfRule type="containsText" dxfId="52" priority="39" operator="containsText" text="literature">
       <formula>NOT(ISERROR(SEARCH("literature",H73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="13" operator="containsText" text="guess">
+    <cfRule type="containsText" dxfId="51" priority="40" operator="containsText" text="guess">
       <formula>NOT(ISERROR(SEARCH("guess",H73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="14" operator="containsText" text="calc">
+    <cfRule type="containsText" dxfId="50" priority="41" operator="containsText" text="calc">
       <formula>NOT(ISERROR(SEARCH("calc",H73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="15" operator="containsText" text="check">
+    <cfRule type="containsText" dxfId="49" priority="42" operator="containsText" text="check">
       <formula>NOT(ISERROR(SEARCH("check",H73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H73:H77">
-    <cfRule type="containsText" dxfId="21" priority="10" operator="containsText" text="internal data">
+    <cfRule type="containsText" dxfId="48" priority="37" operator="containsText" text="internal data">
       <formula>NOT(ISERROR(SEARCH("internal data",H73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D69:J70">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="calc">
+    <cfRule type="containsText" dxfId="47" priority="36" operator="containsText" text="calc">
       <formula>NOT(ISERROR(SEARCH("calc",D69)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69:I70">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="literature">
+    <cfRule type="containsText" dxfId="46" priority="34" operator="containsText" text="literature">
       <formula>NOT(ISERROR(SEARCH("literature",H69)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="guess">
+    <cfRule type="containsText" dxfId="45" priority="35" operator="containsText" text="guess">
       <formula>NOT(ISERROR(SEARCH("guess",H69)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69:I70">
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="not used">
+    <cfRule type="containsText" dxfId="44" priority="29" operator="containsText" text="not used">
       <formula>NOT(ISERROR(SEARCH("not used",H69)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="literature">
+    <cfRule type="containsText" dxfId="43" priority="30" operator="containsText" text="literature">
       <formula>NOT(ISERROR(SEARCH("literature",H69)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="guess">
+    <cfRule type="containsText" dxfId="42" priority="31" operator="containsText" text="guess">
       <formula>NOT(ISERROR(SEARCH("guess",H69)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="calc">
+    <cfRule type="containsText" dxfId="41" priority="32" operator="containsText" text="calc">
       <formula>NOT(ISERROR(SEARCH("calc",H69)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="check">
+    <cfRule type="containsText" dxfId="40" priority="33" operator="containsText" text="check">
       <formula>NOT(ISERROR(SEARCH("check",H69)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H69:H70">
+    <cfRule type="containsText" dxfId="39" priority="28" operator="containsText" text="internal data">
+      <formula>NOT(ISERROR(SEARCH("internal data",H69)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H78">
+    <cfRule type="containsText" dxfId="26" priority="27" operator="containsText" text="calc">
+      <formula>NOT(ISERROR(SEARCH("calc",H78)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H78">
+    <cfRule type="containsText" dxfId="25" priority="25" operator="containsText" text="literature">
+      <formula>NOT(ISERROR(SEARCH("literature",H78)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="guess">
+      <formula>NOT(ISERROR(SEARCH("guess",H78)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H78">
+    <cfRule type="containsText" dxfId="23" priority="20" operator="containsText" text="not used">
+      <formula>NOT(ISERROR(SEARCH("not used",H78)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="21" operator="containsText" text="literature">
+      <formula>NOT(ISERROR(SEARCH("literature",H78)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="guess">
+      <formula>NOT(ISERROR(SEARCH("guess",H78)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="23" operator="containsText" text="calc">
+      <formula>NOT(ISERROR(SEARCH("calc",H78)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="24" operator="containsText" text="check">
+      <formula>NOT(ISERROR(SEARCH("check",H78)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H78">
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="internal data">
+      <formula>NOT(ISERROR(SEARCH("internal data",H78)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H79">
+    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="calc">
+      <formula>NOT(ISERROR(SEARCH("calc",H79)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H79">
+    <cfRule type="containsText" dxfId="16" priority="16" operator="containsText" text="literature">
+      <formula>NOT(ISERROR(SEARCH("literature",H79)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="guess">
+      <formula>NOT(ISERROR(SEARCH("guess",H79)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H79">
+    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="not used">
+      <formula>NOT(ISERROR(SEARCH("not used",H79)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="literature">
+      <formula>NOT(ISERROR(SEARCH("literature",H79)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="guess">
+      <formula>NOT(ISERROR(SEARCH("guess",H79)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="14" operator="containsText" text="calc">
+      <formula>NOT(ISERROR(SEARCH("calc",H79)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="check">
+      <formula>NOT(ISERROR(SEARCH("check",H79)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H79">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="internal data">
+      <formula>NOT(ISERROR(SEARCH("internal data",H79)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H80">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="calc">
+      <formula>NOT(ISERROR(SEARCH("calc",H80)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H80">
+    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="literature">
+      <formula>NOT(ISERROR(SEARCH("literature",H80)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="guess">
+      <formula>NOT(ISERROR(SEARCH("guess",H80)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H80">
+    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="not used">
+      <formula>NOT(ISERROR(SEARCH("not used",H80)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="literature">
+      <formula>NOT(ISERROR(SEARCH("literature",H80)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="guess">
+      <formula>NOT(ISERROR(SEARCH("guess",H80)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="calc">
+      <formula>NOT(ISERROR(SEARCH("calc",H80)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="check">
+      <formula>NOT(ISERROR(SEARCH("check",H80)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H80">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="internal data">
-      <formula>NOT(ISERROR(SEARCH("internal data",H69)))</formula>
+      <formula>NOT(ISERROR(SEARCH("internal data",H80)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>